<commit_message>
updated personnel in excel template
</commit_message>
<xml_diff>
--- a/nes-lter-attune-transect-info.xlsx
+++ b/nes-lter-attune-transect-info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbeaulieu\Desktop\github\nes-lter-attune-transect\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbeaulieu\Desktop\github\nes-lter-attune-transect-continuous\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41ED35DD-8CAF-4EBC-B311-9C97F673E790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5F9CCD4-A8E1-4693-901C-FA85F2EF08BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29085" yWindow="270" windowWidth="23955" windowHeight="20640" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeaders" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="145">
   <si>
     <t>keyword</t>
   </si>
@@ -152,9 +152,6 @@
     <t>Bethany</t>
   </si>
   <si>
-    <t>bfowler@whoi.edu</t>
-  </si>
-  <si>
     <t>0000-0001-8655-7253</t>
   </si>
   <si>
@@ -453,6 +450,15 @@
   </si>
   <si>
     <t>biovolume</t>
+  </si>
+  <si>
+    <t>bstevens@whoi.edu</t>
+  </si>
+  <si>
+    <t>0000-0003-0194-7282</t>
+  </si>
+  <si>
+    <t>0000-0002-2122-0462</t>
   </si>
 </sst>
 </file>
@@ -488,11 +494,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -800,7 +807,7 @@
   </sheetPr>
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
@@ -813,524 +820,524 @@
   <sheetData>
     <row r="1" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>65</v>
-      </c>
       <c r="F3" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>69</v>
-      </c>
       <c r="C4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="F4" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="C5" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="D5" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="F5" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="F6" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="C25" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D25" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="F25" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -1353,30 +1360,30 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1" t="s">
         <v>119</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>120</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>121</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>122</v>
-      </c>
-      <c r="E1" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" t="s">
+        <v>141</v>
+      </c>
+      <c r="E2" t="s">
         <v>124</v>
-      </c>
-      <c r="B2" t="s">
-        <v>142</v>
-      </c>
-      <c r="E2" t="s">
-        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -1396,35 +1403,35 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" t="s">
         <v>88</v>
-      </c>
-      <c r="C1" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -1439,8 +1446,8 @@
   </sheetPr>
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1486,16 +1493,16 @@
         <v>41</v>
       </c>
       <c r="C2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D2" t="s">
         <v>31</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="F2" t="s">
         <v>42</v>
-      </c>
-      <c r="F2" t="s">
-        <v>43</v>
       </c>
       <c r="G2" t="s">
         <v>40</v>
@@ -1544,16 +1551,19 @@
     </row>
     <row r="4" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" t="s">
         <v>44</v>
-      </c>
-      <c r="C4" t="s">
-        <v>45</v>
       </c>
       <c r="D4" t="s">
         <v>31</v>
       </c>
       <c r="E4" t="s">
-        <v>46</v>
+        <v>45</v>
+      </c>
+      <c r="F4" t="s">
+        <v>143</v>
       </c>
       <c r="G4" t="s">
         <v>40</v>
@@ -1581,6 +1591,9 @@
       <c r="E5" t="s">
         <v>39</v>
       </c>
+      <c r="F5" t="s">
+        <v>144</v>
+      </c>
       <c r="G5" t="s">
         <v>40</v>
       </c>
@@ -1628,16 +1641,16 @@
     </row>
     <row r="7" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D7" t="s">
         <v>31</v>
       </c>
       <c r="E7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" t="s">
         <v>48</v>
-      </c>
-      <c r="G7" t="s">
-        <v>49</v>
       </c>
       <c r="H7" t="s">
         <v>31</v>
@@ -1651,19 +1664,19 @@
     </row>
     <row r="8" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" t="s">
         <v>50</v>
-      </c>
-      <c r="C8" t="s">
-        <v>51</v>
       </c>
       <c r="D8" t="s">
         <v>31</v>
       </c>
       <c r="E8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H8" t="s">
         <v>31</v>
@@ -1715,7 +1728,7 @@
     </row>
     <row r="3" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -1755,26 +1768,26 @@
     </row>
     <row r="8" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B8" t="s">
         <v>84</v>
-      </c>
-      <c r="B8" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
revised column headers and methods
</commit_message>
<xml_diff>
--- a/nes-lter-attune-transect-info.xlsx
+++ b/nes-lter-attune-transect-info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sbeaulieu\Desktop\github\nes-lter-attune-transect-continuous\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5F9CCD4-A8E1-4693-901C-FA85F2EF08BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC31E2BF-9D02-43EB-9946-F134A511AF96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29085" yWindow="270" windowWidth="23955" windowHeight="20640" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29160" yWindow="1425" windowWidth="21645" windowHeight="17550" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ColumnHeaders" sheetId="1" r:id="rId1"/>
@@ -323,42 +323,6 @@
     <t>redeuk_leq_20um_cells_per_ml</t>
   </si>
   <si>
-    <t>syn_biovolume</t>
-  </si>
-  <si>
-    <t>redeuk_leq_2um_biovolume</t>
-  </si>
-  <si>
-    <t>redeuk_leq_3um_biovolume</t>
-  </si>
-  <si>
-    <t>redeuk_leq_5um_biovolume</t>
-  </si>
-  <si>
-    <t>redeuk_leq_10um_biovolume</t>
-  </si>
-  <si>
-    <t>redeuk_leq_20um_biovolume</t>
-  </si>
-  <si>
-    <t>syn_carbon</t>
-  </si>
-  <si>
-    <t>redeuk_leq_2um_carbon</t>
-  </si>
-  <si>
-    <t>redeuk_leq_3um_carbon</t>
-  </si>
-  <si>
-    <t>redeuk_leq_5um_carbon</t>
-  </si>
-  <si>
-    <t>redeuk_leq_10um_carbon</t>
-  </si>
-  <si>
-    <t>redeuk_leq_20um_carbon</t>
-  </si>
-  <si>
     <t>depth of underway seawater intake below sea surface http://vocab.nerc.ac.uk/collection/P09/current/DEPH/</t>
   </si>
   <si>
@@ -459,6 +423,42 @@
   </si>
   <si>
     <t>0000-0002-2122-0462</t>
+  </si>
+  <si>
+    <t>syn_biovolume_concentration</t>
+  </si>
+  <si>
+    <t>redeuk_leq_2um_biovolume_concentration</t>
+  </si>
+  <si>
+    <t>redeuk_leq_3um_biovolume_concentration</t>
+  </si>
+  <si>
+    <t>redeuk_leq_5um_biovolume_concentration</t>
+  </si>
+  <si>
+    <t>redeuk_leq_10um_biovolume_concentration</t>
+  </si>
+  <si>
+    <t>redeuk_leq_20um_biovolume_concentration</t>
+  </si>
+  <si>
+    <t>syn_carbon_concentration</t>
+  </si>
+  <si>
+    <t>redeuk_leq_2um_carbon_concentration</t>
+  </si>
+  <si>
+    <t>redeuk_leq_3um_carbon_concentration</t>
+  </si>
+  <si>
+    <t>redeuk_leq_5um_carbon_concentration</t>
+  </si>
+  <si>
+    <t>redeuk_leq_10um_carbon_concentration</t>
+  </si>
+  <si>
+    <t>redeuk_leq_20um_carbon_concentration</t>
   </si>
 </sst>
 </file>
@@ -494,12 +494,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -807,8 +806,8 @@
   </sheetPr>
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -917,7 +916,7 @@
         <v>73</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>69</v>
@@ -937,7 +936,7 @@
         <v>93</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>69</v>
@@ -957,7 +956,7 @@
         <v>94</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>69</v>
@@ -977,7 +976,7 @@
         <v>95</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>69</v>
@@ -997,7 +996,7 @@
         <v>96</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>69</v>
@@ -1017,7 +1016,7 @@
         <v>97</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>69</v>
@@ -1037,7 +1036,7 @@
         <v>98</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>69</v>
@@ -1054,16 +1053,16 @@
     </row>
     <row r="13" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>99</v>
+        <v>133</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>69</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>65</v>
@@ -1074,16 +1073,16 @@
     </row>
     <row r="14" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>100</v>
+        <v>134</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>69</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>65</v>
@@ -1094,16 +1093,16 @@
     </row>
     <row r="15" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>101</v>
+        <v>135</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>69</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>65</v>
@@ -1114,16 +1113,16 @@
     </row>
     <row r="16" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>102</v>
+        <v>136</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>69</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>65</v>
@@ -1134,16 +1133,16 @@
     </row>
     <row r="17" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>103</v>
+        <v>137</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>69</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>65</v>
@@ -1154,16 +1153,16 @@
     </row>
     <row r="18" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>104</v>
+        <v>138</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>69</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>65</v>
@@ -1174,16 +1173,16 @@
     </row>
     <row r="19" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>105</v>
+        <v>139</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>69</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>65</v>
@@ -1194,16 +1193,16 @@
     </row>
     <row r="20" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>106</v>
+        <v>140</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>69</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>65</v>
@@ -1214,16 +1213,16 @@
     </row>
     <row r="21" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>107</v>
+        <v>141</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>69</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>65</v>
@@ -1234,16 +1233,16 @@
     </row>
     <row r="22" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>108</v>
+        <v>142</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>69</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>65</v>
@@ -1254,16 +1253,16 @@
     </row>
     <row r="23" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>109</v>
+        <v>143</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>69</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>65</v>
@@ -1274,16 +1273,16 @@
     </row>
     <row r="24" spans="1:7" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>110</v>
+        <v>144</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>69</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>65</v>
@@ -1317,7 +1316,7 @@
         <v>79</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>61</v>
@@ -1334,10 +1333,10 @@
         <v>89</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -1360,30 +1359,30 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
       <c r="B1" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="C1" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="D1" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="E1" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="B2" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="E2" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -1446,7 +1445,7 @@
   </sheetPr>
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
@@ -1498,8 +1497,8 @@
       <c r="D2" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>142</v>
+      <c r="E2" t="s">
+        <v>130</v>
       </c>
       <c r="F2" t="s">
         <v>42</v>
@@ -1563,7 +1562,7 @@
         <v>45</v>
       </c>
       <c r="F4" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="G4" t="s">
         <v>40</v>
@@ -1592,7 +1591,7 @@
         <v>39</v>
       </c>
       <c r="F5" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="G5" t="s">
         <v>40</v>

</xml_diff>